<commit_message>
Third tab more or less complete, I'm still having issues with sizing and stacking.
</commit_message>
<xml_diff>
--- a/finalproject/raw-data/Crime Rate + Pop.xlsx
+++ b/finalproject/raw-data/Crime Rate + Pop.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophia/Documents/Grad School/GOV 1005/Final Project/New project/Data/Cleaned Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophia/Desktop/R Projects/final-project/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E90BD06-BE9B-444A-A23C-C12E2A324F20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402B97F0-3C88-8448-A293-063858A635DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4280" yWindow="460" windowWidth="23200" windowHeight="17040" xr2:uid="{312A87DE-AC3C-C342-8421-52458E24D9E0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Year</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>PopulationPPB</t>
+  </si>
+  <si>
+    <t>PopulationCen</t>
   </si>
 </sst>
 </file>
@@ -394,22 +397,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB48161B-2AAD-3243-90EB-C97B3A4B4B93}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,19 +421,22 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -437,19 +444,22 @@
         <v>583775</v>
       </c>
       <c r="C2">
+        <v>585436</v>
+      </c>
+      <c r="D2">
         <v>3090</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>5.3</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>28549</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>48.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -457,19 +467,22 @@
         <v>585845</v>
       </c>
       <c r="C3">
+        <v>595410</v>
+      </c>
+      <c r="D3">
         <v>3000</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>29994</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>51.2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -477,19 +490,22 @@
         <v>587865</v>
       </c>
       <c r="C4">
+        <v>604285</v>
+      </c>
+      <c r="D4">
         <v>3156</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>5.4</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>30773</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>52.3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -497,19 +513,22 @@
         <v>592120</v>
       </c>
       <c r="C5">
+        <v>609970</v>
+      </c>
+      <c r="D5">
         <v>2979</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>29648</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>50.1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -517,19 +536,22 @@
         <v>601510</v>
       </c>
       <c r="C6">
+        <v>620647</v>
+      </c>
+      <c r="D6">
         <v>2920</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>32232</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>53.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -537,19 +559,22 @@
         <v>613355</v>
       </c>
       <c r="C7">
+        <v>631539</v>
+      </c>
+      <c r="D7">
         <v>3002</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>31973</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>52.1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -557,19 +582,22 @@
         <v>627395</v>
       </c>
       <c r="C8">
+        <v>643136</v>
+      </c>
+      <c r="D8">
         <v>3251</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>5.2</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>33324</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>53.1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -577,19 +605,22 @@
         <v>639100</v>
       </c>
       <c r="C9">
+        <v>648630</v>
+      </c>
+      <c r="D9">
         <v>3418</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>5.3</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>36556</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>57.2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -597,15 +628,18 @@
         <v>648740</v>
       </c>
       <c r="C10">
+        <v>643115</v>
+      </c>
+      <c r="D10">
         <v>3521</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>5.4</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>35861</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>55.3</v>
       </c>
     </row>

</xml_diff>